<commit_message>
add both SN ratio table
</commit_message>
<xml_diff>
--- a/AIIoU SN Ratio.xlsx
+++ b/AIIoU SN Ratio.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\61452\Desktop\Carbon-Fiber-Detection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D435280-308A-4512-B40A-0D022A8D95E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A0A0DF8-6B0B-43A1-9621-0A559BFC25CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2940" yWindow="288" windowWidth="12456" windowHeight="11424" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="13">
   <si>
     <t>Group</t>
   </si>
@@ -34,9 +47,6 @@
     <t>Fibre Feed Rate</t>
   </si>
   <si>
-    <t>Nylon Feed rate</t>
-  </si>
-  <si>
     <t>Radius 2.5</t>
   </si>
   <si>
@@ -45,12 +55,30 @@
   <si>
     <t>Radius 10</t>
   </si>
+  <si>
+    <t>Level 2</t>
+  </si>
+  <si>
+    <t>Level 1</t>
+  </si>
+  <si>
+    <t>Level 3</t>
+  </si>
+  <si>
+    <t>Level 4</t>
+  </si>
+  <si>
+    <t>Nylon Feed Rate</t>
+  </si>
+  <si>
+    <t>Range</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -66,6 +94,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -75,7 +109,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -98,14 +132,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -445,15 +496,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -467,19 +518,19 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -504,8 +555,13 @@
       <c r="H2">
         <v>0.67734748044149129</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -528,10 +584,10 @@
         <v>0.83995471674363709</v>
       </c>
       <c r="H3">
-        <v>0.66338587836048979</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+        <v>0.66338587836049001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -557,7 +613,7 @@
         <v>1.529162614259054</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -583,7 +639,7 @@
         <v>2.5443276893765958</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -609,7 +665,7 @@
         <v>0.99543472544403477</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -635,7 +691,7 @@
         <v>0.58805177341257764</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -660,8 +716,13 @@
       <c r="H8">
         <v>2.8141814018967568</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -687,7 +748,7 @@
         <v>0.95198088248163182</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -713,7 +774,7 @@
         <v>1.78700538368962</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -739,7 +800,7 @@
         <v>3.207583511862802</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -765,7 +826,7 @@
         <v>0.1782409184711278</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -791,7 +852,7 @@
         <v>0.57224983260276729</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -816,8 +877,13 @@
       <c r="H14">
         <v>3.3825438246544861</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -843,7 +909,7 @@
         <v>1.904724538433487</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -898,4 +964,371 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{118319DD-C9A5-40D7-962C-99A517E0A0CF}">
+  <dimension ref="A1:F15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <v>1.3535559156093999</v>
+      </c>
+      <c r="C2" s="3">
+        <v>1.3374121958087499</v>
+      </c>
+      <c r="D2" s="3">
+        <v>1.43626991165657</v>
+      </c>
+      <c r="E2" s="3">
+        <v>1.5193142616292801</v>
+      </c>
+      <c r="F2">
+        <f>MAX(B2:E2)-MIN(B2:E2)</f>
+        <v>0.18190206582053015</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>1.7105828535573999</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1.5909364255173299</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1.2575055029464099</v>
+      </c>
+      <c r="E3" s="3">
+        <v>1.0875275026828599</v>
+      </c>
+      <c r="F3">
+        <f>MAX(B3:E3)-MIN(B3:E3)</f>
+        <v>0.62305535087454</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.43129794464891302</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.68487687839150402</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1.5432183547159399</v>
+      </c>
+      <c r="E4" s="3">
+        <v>2.9871591069476602</v>
+      </c>
+      <c r="F4">
+        <f>MAX(B4:E4)-MIN(B4:E4)</f>
+        <v>2.555861162298747</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="3">
+        <v>1.4921258133436199</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1.29403787599193</v>
+      </c>
+      <c r="D5" s="3">
+        <v>1.50343311445908</v>
+      </c>
+      <c r="E5" s="3">
+        <v>1.35695548090937</v>
+      </c>
+      <c r="F5">
+        <f>MAX(B5:E5)-MIN(B5:E5)</f>
+        <v>0.20939523846715002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="3">
+        <v>1.0926474063404901</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.88141317380928597</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0.95054081228788501</v>
+      </c>
+      <c r="E7" s="3">
+        <v>1.0010880403591</v>
+      </c>
+      <c r="F7">
+        <f>MAX(B7:E7)-MIN(B7:E7)</f>
+        <v>0.2112342325312041</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="3">
+        <v>1.04142799615238</v>
+      </c>
+      <c r="C8" s="3">
+        <v>1.1183167697793599</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1.0017744168529601</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0.76417025001205496</v>
+      </c>
+      <c r="F8">
+        <f>MAX(B8:E8)-MIN(B8:E8)</f>
+        <v>0.35414651976730493</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.34158432194746302</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0.53024971846365798</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1.11282384432305</v>
+      </c>
+      <c r="E9" s="3">
+        <v>1.9410315480625899</v>
+      </c>
+      <c r="F9">
+        <f>MAX(B9:E9)-MIN(B9:E9)</f>
+        <v>1.5994472261151269</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="3">
+        <v>1.0104391186603101</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0.97898132132387405</v>
+      </c>
+      <c r="D10" s="3">
+        <v>1.04001251485827</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0.89625647795430197</v>
+      </c>
+      <c r="F10">
+        <f>MAX(B10:E10)-MIN(B10:E10)</f>
+        <v>0.14375603690396799</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="3">
+        <v>0.389213795048794</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0.117445242229773</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0.30862192355269302</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0.42788287650562601</v>
+      </c>
+      <c r="F12">
+        <f>MAX(B12:E12)-MIN(B12:E12)</f>
+        <v>0.31043763427585302</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="3">
+        <v>0.48541900718783498</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0.28082675103204202</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0.164800447911406</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0.31211763120560199</v>
+      </c>
+      <c r="F13">
+        <f>MAX(B13:E13)-MIN(B13:E13)</f>
+        <v>0.32061855927642902</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="3">
+        <v>5.87742019247064E-2</v>
+      </c>
+      <c r="C14" s="3">
+        <v>9.2481203408544599E-2</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0.21920613003476999</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0.872702301968866</v>
+      </c>
+      <c r="F14">
+        <f>MAX(B14:E14)-MIN(B14:E14)</f>
+        <v>0.81392810004415961</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="3">
+        <v>0.194410279736834</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0.41650424570384098</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0.26150328698631198</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0.370746024909898</v>
+      </c>
+      <c r="F15">
+        <f>MAX(B15:E15)-MIN(B15:E15)</f>
+        <v>0.22209396596700698</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B7:E10">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B12:E15">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:E5">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add overall sn ratio
</commit_message>
<xml_diff>
--- a/AIIoU SN Ratio.xlsx
+++ b/AIIoU SN Ratio.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\61452\Desktop\Carbon-Fiber-Detection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A0A0DF8-6B0B-43A1-9621-0A559BFC25CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDCB37E2-B694-431C-AA9B-DA7E610285B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2940" yWindow="288" windowWidth="12456" windowHeight="11424" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16332" yWindow="2856" windowWidth="15360" windowHeight="11292" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
+    <sheet name="SN Ratio" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="16">
   <si>
     <t>Group</t>
   </si>
@@ -72,6 +73,15 @@
   </si>
   <si>
     <t>Range</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>SN ratio</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -147,7 +157,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -157,6 +167,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -499,7 +512,7 @@
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:E17"/>
+      <selection sqref="A1:H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -967,11 +980,1153 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48C25B17-5B73-4322-9094-5AA61AFC9CA8}">
+  <dimension ref="A1:G49"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>240</v>
+      </c>
+      <c r="C2">
+        <v>120</v>
+      </c>
+      <c r="D2">
+        <v>0.8</v>
+      </c>
+      <c r="E2">
+        <v>0.6</v>
+      </c>
+      <c r="F2">
+        <v>0.67734748044149129</v>
+      </c>
+      <c r="G2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>240</v>
+      </c>
+      <c r="C3">
+        <v>280</v>
+      </c>
+      <c r="D3">
+        <v>0.9</v>
+      </c>
+      <c r="E3">
+        <v>0.8</v>
+      </c>
+      <c r="F3">
+        <v>0.66338587836049001</v>
+      </c>
+      <c r="G3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>240</v>
+      </c>
+      <c r="C4">
+        <v>440</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1.529162614259054</v>
+      </c>
+      <c r="G4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>240</v>
+      </c>
+      <c r="C5">
+        <v>600</v>
+      </c>
+      <c r="D5">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E5">
+        <v>1.2</v>
+      </c>
+      <c r="F5">
+        <v>2.5443276893765958</v>
+      </c>
+      <c r="G5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>250</v>
+      </c>
+      <c r="C6">
+        <v>120</v>
+      </c>
+      <c r="D6">
+        <v>0.9</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>0.99543472544403477</v>
+      </c>
+      <c r="G6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>250</v>
+      </c>
+      <c r="C7">
+        <v>280</v>
+      </c>
+      <c r="D7">
+        <v>0.8</v>
+      </c>
+      <c r="E7">
+        <v>1.2</v>
+      </c>
+      <c r="F7">
+        <v>0.58805177341257764</v>
+      </c>
+      <c r="G7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>250</v>
+      </c>
+      <c r="C8">
+        <v>440</v>
+      </c>
+      <c r="D8">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E8">
+        <v>0.6</v>
+      </c>
+      <c r="F8">
+        <v>2.8141814018967568</v>
+      </c>
+      <c r="G8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>250</v>
+      </c>
+      <c r="C9">
+        <v>600</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>0.8</v>
+      </c>
+      <c r="F9">
+        <v>0.95198088248163182</v>
+      </c>
+      <c r="G9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>260</v>
+      </c>
+      <c r="C10">
+        <v>120</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>1.2</v>
+      </c>
+      <c r="F10">
+        <v>1.78700538368962</v>
+      </c>
+      <c r="G10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>260</v>
+      </c>
+      <c r="C11">
+        <v>280</v>
+      </c>
+      <c r="D11">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>3.207583511862802</v>
+      </c>
+      <c r="G11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>260</v>
+      </c>
+      <c r="C12">
+        <v>440</v>
+      </c>
+      <c r="D12">
+        <v>0.8</v>
+      </c>
+      <c r="E12">
+        <v>0.8</v>
+      </c>
+      <c r="F12">
+        <v>0.1782409184711278</v>
+      </c>
+      <c r="G12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>260</v>
+      </c>
+      <c r="C13">
+        <v>600</v>
+      </c>
+      <c r="D13">
+        <v>0.9</v>
+      </c>
+      <c r="E13">
+        <v>0.6</v>
+      </c>
+      <c r="F13">
+        <v>0.57224983260276729</v>
+      </c>
+      <c r="G13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>270</v>
+      </c>
+      <c r="C14">
+        <v>120</v>
+      </c>
+      <c r="D14">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E14">
+        <v>0.8</v>
+      </c>
+      <c r="F14">
+        <v>3.3825438246544861</v>
+      </c>
+      <c r="G14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>270</v>
+      </c>
+      <c r="C15">
+        <v>280</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>0.6</v>
+      </c>
+      <c r="F15">
+        <v>1.904724538433487</v>
+      </c>
+      <c r="G15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>270</v>
+      </c>
+      <c r="C16">
+        <v>440</v>
+      </c>
+      <c r="D16">
+        <v>0.9</v>
+      </c>
+      <c r="E16">
+        <v>1.2</v>
+      </c>
+      <c r="F16">
+        <v>0.50843707715872555</v>
+      </c>
+      <c r="G16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>270</v>
+      </c>
+      <c r="C17">
+        <v>600</v>
+      </c>
+      <c r="D17">
+        <v>0.8</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>0.2815516062704555</v>
+      </c>
+      <c r="G17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18">
+        <v>240</v>
+      </c>
+      <c r="C18">
+        <v>120</v>
+      </c>
+      <c r="D18">
+        <v>0.8</v>
+      </c>
+      <c r="E18">
+        <v>0.6</v>
+      </c>
+      <c r="F18">
+        <v>0.40316453022880011</v>
+      </c>
+      <c r="G18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>2</v>
+      </c>
+      <c r="B19">
+        <v>240</v>
+      </c>
+      <c r="C19">
+        <v>280</v>
+      </c>
+      <c r="D19">
+        <v>0.9</v>
+      </c>
+      <c r="E19">
+        <v>0.8</v>
+      </c>
+      <c r="F19">
+        <v>0.83995471674363709</v>
+      </c>
+      <c r="G19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>3</v>
+      </c>
+      <c r="B20">
+        <v>240</v>
+      </c>
+      <c r="C20">
+        <v>440</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>1.3813534396196341</v>
+      </c>
+      <c r="G20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>4</v>
+      </c>
+      <c r="B21">
+        <v>240</v>
+      </c>
+      <c r="C21">
+        <v>600</v>
+      </c>
+      <c r="D21">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E21">
+        <v>1.2</v>
+      </c>
+      <c r="F21">
+        <v>1.746116938769922</v>
+      </c>
+      <c r="G21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>5</v>
+      </c>
+      <c r="B22">
+        <v>250</v>
+      </c>
+      <c r="C22">
+        <v>120</v>
+      </c>
+      <c r="D22">
+        <v>0.9</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>0.54511465968407768</v>
+      </c>
+      <c r="G22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>6</v>
+      </c>
+      <c r="B23">
+        <v>250</v>
+      </c>
+      <c r="C23">
+        <v>280</v>
+      </c>
+      <c r="D23">
+        <v>0.8</v>
+      </c>
+      <c r="E23">
+        <v>1.2</v>
+      </c>
+      <c r="F23">
+        <v>0.3716660007352493</v>
+      </c>
+      <c r="G23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>7</v>
+      </c>
+      <c r="B24">
+        <v>250</v>
+      </c>
+      <c r="C24">
+        <v>440</v>
+      </c>
+      <c r="D24">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E24">
+        <v>0.6</v>
+      </c>
+      <c r="F24">
+        <v>1.9544177582214131</v>
+      </c>
+      <c r="G24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>8</v>
+      </c>
+      <c r="B25">
+        <v>250</v>
+      </c>
+      <c r="C25">
+        <v>600</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>0.8</v>
+      </c>
+      <c r="F25">
+        <v>0.65445427659640432</v>
+      </c>
+      <c r="G25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>9</v>
+      </c>
+      <c r="B26">
+        <v>260</v>
+      </c>
+      <c r="C26">
+        <v>120</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>1.2</v>
+      </c>
+      <c r="F26">
+        <v>1.1208086315538719</v>
+      </c>
+      <c r="G26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>10</v>
+      </c>
+      <c r="B27">
+        <v>260</v>
+      </c>
+      <c r="C27">
+        <v>280</v>
+      </c>
+      <c r="D27">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <v>1.966967332116256</v>
+      </c>
+      <c r="G27">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>11</v>
+      </c>
+      <c r="B28">
+        <v>260</v>
+      </c>
+      <c r="C28">
+        <v>440</v>
+      </c>
+      <c r="D28">
+        <v>0.8</v>
+      </c>
+      <c r="E28">
+        <v>0.8</v>
+      </c>
+      <c r="F28">
+        <v>0.32489212881266172</v>
+      </c>
+      <c r="G28">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>12</v>
+      </c>
+      <c r="B29">
+        <v>260</v>
+      </c>
+      <c r="C29">
+        <v>600</v>
+      </c>
+      <c r="D29">
+        <v>0.9</v>
+      </c>
+      <c r="E29">
+        <v>0.6</v>
+      </c>
+      <c r="F29">
+        <v>0.38949515666875262</v>
+      </c>
+      <c r="G29">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>13</v>
+      </c>
+      <c r="B30">
+        <v>270</v>
+      </c>
+      <c r="C30">
+        <v>120</v>
+      </c>
+      <c r="D30">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E30">
+        <v>0.8</v>
+      </c>
+      <c r="F30">
+        <v>2.0966241631427969</v>
+      </c>
+      <c r="G30">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>14</v>
+      </c>
+      <c r="B31">
+        <v>270</v>
+      </c>
+      <c r="C31">
+        <v>280</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>0.6</v>
+      </c>
+      <c r="F31">
+        <v>1.2946790295223061</v>
+      </c>
+      <c r="G31">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>15</v>
+      </c>
+      <c r="B32">
+        <v>270</v>
+      </c>
+      <c r="C32">
+        <v>440</v>
+      </c>
+      <c r="D32">
+        <v>0.9</v>
+      </c>
+      <c r="E32">
+        <v>1.2</v>
+      </c>
+      <c r="F32">
+        <v>0.34643434075816609</v>
+      </c>
+      <c r="G32">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>16</v>
+      </c>
+      <c r="B33">
+        <v>270</v>
+      </c>
+      <c r="C33">
+        <v>600</v>
+      </c>
+      <c r="D33">
+        <v>0.8</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33">
+        <v>0.26661462801314101</v>
+      </c>
+      <c r="G33">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>1</v>
+      </c>
+      <c r="B34">
+        <v>240</v>
+      </c>
+      <c r="C34">
+        <v>120</v>
+      </c>
+      <c r="D34">
+        <v>0.8</v>
+      </c>
+      <c r="E34">
+        <v>0.6</v>
+      </c>
+      <c r="F34">
+        <v>0.17523987826640999</v>
+      </c>
+      <c r="G34">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>2</v>
+      </c>
+      <c r="B35">
+        <v>240</v>
+      </c>
+      <c r="C35">
+        <v>280</v>
+      </c>
+      <c r="D35">
+        <v>0.9</v>
+      </c>
+      <c r="E35">
+        <v>0.8</v>
+      </c>
+      <c r="F35">
+        <v>0.1187479985709745</v>
+      </c>
+      <c r="G35">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>3</v>
+      </c>
+      <c r="B36">
+        <v>240</v>
+      </c>
+      <c r="C36">
+        <v>440</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="F36">
+        <v>0.25178667809021632</v>
+      </c>
+      <c r="G36">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>4</v>
+      </c>
+      <c r="B37">
+        <v>240</v>
+      </c>
+      <c r="C37">
+        <v>600</v>
+      </c>
+      <c r="D37">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E37">
+        <v>1.2</v>
+      </c>
+      <c r="F37">
+        <v>1.011080625267577</v>
+      </c>
+      <c r="G37">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>5</v>
+      </c>
+      <c r="B38">
+        <v>250</v>
+      </c>
+      <c r="C38">
+        <v>120</v>
+      </c>
+      <c r="D38">
+        <v>0.9</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="F38">
+        <v>2.3149611946881511E-2</v>
+      </c>
+      <c r="G38">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>6</v>
+      </c>
+      <c r="B39">
+        <v>250</v>
+      </c>
+      <c r="C39">
+        <v>280</v>
+      </c>
+      <c r="D39">
+        <v>0.8</v>
+      </c>
+      <c r="E39">
+        <v>1.2</v>
+      </c>
+      <c r="F39">
+        <v>4.4855238205353559E-2</v>
+      </c>
+      <c r="G39">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>7</v>
+      </c>
+      <c r="B40">
+        <v>250</v>
+      </c>
+      <c r="C40">
+        <v>440</v>
+      </c>
+      <c r="D40">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E40">
+        <v>0.6</v>
+      </c>
+      <c r="F40">
+        <v>0.28908027522463148</v>
+      </c>
+      <c r="G40">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>8</v>
+      </c>
+      <c r="B41">
+        <v>250</v>
+      </c>
+      <c r="C41">
+        <v>600</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41">
+        <v>0.8</v>
+      </c>
+      <c r="F41">
+        <v>0.1126958435422266</v>
+      </c>
+      <c r="G41">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>9</v>
+      </c>
+      <c r="B42">
+        <v>260</v>
+      </c>
+      <c r="C42">
+        <v>120</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42">
+        <v>1.2</v>
+      </c>
+      <c r="F42">
+        <v>0.32371508906294921</v>
+      </c>
+      <c r="G42">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>10</v>
+      </c>
+      <c r="B43">
+        <v>260</v>
+      </c>
+      <c r="C43">
+        <v>280</v>
+      </c>
+      <c r="D43">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E43">
+        <v>1</v>
+      </c>
+      <c r="F43">
+        <v>0.77107685790815328</v>
+      </c>
+      <c r="G43">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>11</v>
+      </c>
+      <c r="B44">
+        <v>260</v>
+      </c>
+      <c r="C44">
+        <v>440</v>
+      </c>
+      <c r="D44">
+        <v>0.8</v>
+      </c>
+      <c r="E44">
+        <v>0.8</v>
+      </c>
+      <c r="F44">
+        <v>1.5001691227062099E-2</v>
+      </c>
+      <c r="G44">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>12</v>
+      </c>
+      <c r="B45">
+        <v>260</v>
+      </c>
+      <c r="C45">
+        <v>600</v>
+      </c>
+      <c r="D45">
+        <v>0.9</v>
+      </c>
+      <c r="E45">
+        <v>0.6</v>
+      </c>
+      <c r="F45">
+        <v>0.1246940560126082</v>
+      </c>
+      <c r="G45">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>13</v>
+      </c>
+      <c r="B46">
+        <v>270</v>
+      </c>
+      <c r="C46">
+        <v>120</v>
+      </c>
+      <c r="D46">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E46">
+        <v>0.8</v>
+      </c>
+      <c r="F46">
+        <v>1.4195714494751019</v>
+      </c>
+      <c r="G46">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>14</v>
+      </c>
+      <c r="B47">
+        <v>270</v>
+      </c>
+      <c r="C47">
+        <v>280</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="E47">
+        <v>0.6</v>
+      </c>
+      <c r="F47">
+        <v>0.18862690944368801</v>
+      </c>
+      <c r="G47">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>15</v>
+      </c>
+      <c r="B48">
+        <v>270</v>
+      </c>
+      <c r="C48">
+        <v>440</v>
+      </c>
+      <c r="D48">
+        <v>0.9</v>
+      </c>
+      <c r="E48">
+        <v>1.2</v>
+      </c>
+      <c r="F48">
+        <v>0.1033331471037145</v>
+      </c>
+      <c r="G48">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>16</v>
+      </c>
+      <c r="B49">
+        <v>270</v>
+      </c>
+      <c r="C49">
+        <v>600</v>
+      </c>
+      <c r="D49">
+        <v>0.8</v>
+      </c>
+      <c r="E49">
+        <v>1</v>
+      </c>
+      <c r="F49">
+        <v>0</v>
+      </c>
+      <c r="G49">
+        <v>2.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{118319DD-C9A5-40D7-962C-99A517E0A0CF}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1291,8 +2446,136 @@
         <v>0.22209396596700698</v>
       </c>
     </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="3">
+        <v>0.94513903899956597</v>
+      </c>
+      <c r="C17" s="3">
+        <v>0.77875687061593601</v>
+      </c>
+      <c r="D17" s="3">
+        <v>0.89847754916571898</v>
+      </c>
+      <c r="E17" s="3">
+        <v>0.98276172616467194</v>
+      </c>
+      <c r="F17">
+        <f>MAX(B17:E17)-MIN(B17:E17)</f>
+        <v>0.20400485554873593</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" s="3">
+        <v>1.07914328563254</v>
+      </c>
+      <c r="C18" s="3">
+        <v>0.99669331544291395</v>
+      </c>
+      <c r="D18" s="3">
+        <v>0.80802678923693005</v>
+      </c>
+      <c r="E18" s="3">
+        <v>0.72127179463350599</v>
+      </c>
+      <c r="F18">
+        <f>MAX(B18:E18)-MIN(B18:E18)</f>
+        <v>0.35787149099903404</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="3">
+        <v>0.27721882284035998</v>
+      </c>
+      <c r="C19" s="3">
+        <v>0.435869266754569</v>
+      </c>
+      <c r="D19" s="3">
+        <v>0.95841610969125701</v>
+      </c>
+      <c r="E19" s="3">
+        <v>1.9336309856597</v>
+      </c>
+      <c r="F19">
+        <f>MAX(B19:E19)-MIN(B19:E19)</f>
+        <v>1.65641216281934</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" s="3">
+        <v>0.89899173724692505</v>
+      </c>
+      <c r="C20" s="3">
+        <v>0.89650781433988302</v>
+      </c>
+      <c r="D20" s="3">
+        <v>0.93498297210122505</v>
+      </c>
+      <c r="E20" s="3">
+        <v>0.87465266125786001</v>
+      </c>
+      <c r="F20">
+        <f>MAX(B20:E20)-MIN(B20:E20)</f>
+        <v>6.0330310843365043E-2</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="B7:E10">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B12:E15">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:E5">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -1304,19 +2587,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B12:E15">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2:E5">
+  <conditionalFormatting sqref="B17:E20">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>